<commit_message>
Added code for Graded Cover
</commit_message>
<xml_diff>
--- a/com.absli.auto/src/main/java/com/absli/testdata/Master Policy Maker - Test Data.xlsx
+++ b/com.absli.auto/src/main/java/com/absli/testdata/Master Policy Maker - Test Data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulnath\eclipse-workspace\com.absli.auto\src\main\java\com\absli\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gokulnath\git\com.absli.auto\com.absli.auto\src\main\java\com\absli\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TC_MPM_001" sheetId="1" r:id="rId1"/>
     <sheet name="TC_MPM_002" sheetId="2" r:id="rId2"/>
     <sheet name="TC_MPM_003" sheetId="3" r:id="rId3"/>
+    <sheet name="TC_MPM_004" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="84">
   <si>
     <t>Client Name</t>
   </si>
@@ -413,6 +414,222 @@
   </si>
   <si>
     <t>Flat Sum Assured</t>
+  </si>
+  <si>
+    <t>Graded Cover</t>
+  </si>
+  <si>
+    <t>Grade 1</t>
+  </si>
+  <si>
+    <t>Grade 3</t>
+  </si>
+  <si>
+    <t>Grade 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sum Assured
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Free Cover Limit (Sum Assured)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Minimum Cap
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maximum Cap 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sum Assured
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Free Cover Limit (Sum Assured)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Minimum Cap
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maximum Cap 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sum Assured
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Free Cover Limit (Sum Assured)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Minimum Cap
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maximum Cap 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Grade 3)</t>
+    </r>
+  </si>
+  <si>
+    <t>10000000</t>
+  </si>
+  <si>
+    <t>5000000</t>
+  </si>
+  <si>
+    <t>2000000</t>
+  </si>
+  <si>
+    <t>3000000</t>
   </si>
 </sst>
 </file>
@@ -823,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
@@ -1302,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,4 +1768,333 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM6" sqref="AM6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="24" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" customWidth="1"/>
+    <col min="19" max="19" width="18.85546875" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" customWidth="1"/>
+    <col min="21" max="21" width="18" customWidth="1"/>
+    <col min="22" max="22" width="19.7109375" customWidth="1"/>
+    <col min="23" max="23" width="31.28515625" customWidth="1"/>
+    <col min="26" max="26" width="24" customWidth="1"/>
+    <col min="27" max="27" width="20.5703125" customWidth="1"/>
+    <col min="28" max="28" width="17" customWidth="1"/>
+    <col min="29" max="29" width="52.7109375" customWidth="1"/>
+    <col min="30" max="30" width="46.85546875" customWidth="1"/>
+    <col min="31" max="31" width="12.5703125" customWidth="1"/>
+    <col min="32" max="32" width="20.28515625" customWidth="1"/>
+    <col min="33" max="33" width="17.5703125" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" customWidth="1"/>
+    <col min="35" max="35" width="17.28515625" customWidth="1"/>
+    <col min="37" max="37" width="18.85546875" customWidth="1"/>
+    <col min="38" max="38" width="26.28515625" customWidth="1"/>
+    <col min="39" max="39" width="20.28515625" customWidth="1"/>
+    <col min="40" max="40" width="16.5703125" customWidth="1"/>
+    <col min="42" max="42" width="20.7109375" customWidth="1"/>
+    <col min="43" max="43" width="26" customWidth="1"/>
+    <col min="44" max="44" width="16" customWidth="1"/>
+    <col min="45" max="45" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:45" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3">
+        <v>132413</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="3">
+        <v>9489466321</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="7">
+        <v>45323</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="3">
+        <v>17</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS2" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>